<commit_message>
ready to test how to write on the table, getting data ok , need to test some more and refactor the functions
</commit_message>
<xml_diff>
--- a/files/A01-101 APT Agar.xlsx
+++ b/files/A01-101 APT Agar.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5B2D965-CDFE-4C46-B420-9906341393FE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D1FADF-44DF-4F89-8BFF-55D83A6B82CB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="420" windowWidth="15465" windowHeight="11025"/>
+    <workbookView xWindow="32760" yWindow="420" windowWidth="15465" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory Master" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="193">
   <si>
     <t>.</t>
   </si>
@@ -620,18 +620,34 @@
   <si>
     <t>Bulk-Other</t>
   </si>
+  <si>
+    <t>3M 2.5 kg 
+70200789033</t>
+  </si>
+  <si>
+    <t>A01-101-E</t>
+  </si>
+  <si>
+    <t>A01-101-N</t>
+  </si>
+  <si>
+    <t>MS-1020-6</t>
+  </si>
+  <si>
+    <t>70-2007-8903-3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -756,12 +772,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1262,7 +1272,7 @@
     <xf numFmtId="0" fontId="22" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="20" fillId="18" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="20" fillId="18" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="7" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1283,8 +1293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1298,6 +1307,9 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1637,14 +1649,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF00FF"/>
   </sheetPr>
   <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1653,7 +1665,9 @@
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" customWidth="1"/>
+    <col min="9" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1679,13 +1693,24 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>189</v>
+      </c>
       <c r="D3" t="s">
         <v>183</v>
       </c>
       <c r="E3" s="161" t="s">
         <v>186</v>
       </c>
-      <c r="H3" s="162"/>
+      <c r="F3" t="s">
+        <v>190</v>
+      </c>
+      <c r="G3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H3" t="s">
+        <v>192</v>
+      </c>
       <c r="L3" s="51" t="s">
         <v>185</v>
       </c>
@@ -1715,8 +1740,8 @@
       <c r="G4" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>9</v>
+      <c r="H4" s="167" t="s">
+        <v>188</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>9</v>
@@ -2837,15 +2862,15 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF00FF"/>
   </sheetPr>
   <dimension ref="A1:T83"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2883,13 +2908,13 @@
       <c r="K2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
-      <c r="P2" s="163"/>
-      <c r="Q2" s="163"/>
-      <c r="R2" s="163"/>
-      <c r="S2" s="163"/>
-      <c r="T2" s="163"/>
+      <c r="N2" s="162"/>
+      <c r="O2" s="162"/>
+      <c r="P2" s="162"/>
+      <c r="Q2" s="162"/>
+      <c r="R2" s="162"/>
+      <c r="S2" s="162"/>
+      <c r="T2" s="162"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
@@ -2900,10 +2925,10 @@
       </c>
     </row>
     <row r="4" spans="1:20" s="149" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="164" t="s">
+      <c r="A4" s="163" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="164"/>
+      <c r="B4" s="163"/>
     </row>
     <row r="5" spans="1:20" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="97" t="s">
@@ -3482,7 +3507,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF00FF"/>
   </sheetPr>
@@ -3529,13 +3554,13 @@
       <c r="K2" s="117">
         <v>161228021912</v>
       </c>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
-      <c r="P2" s="163"/>
-      <c r="Q2" s="163"/>
-      <c r="R2" s="163"/>
-      <c r="S2" s="163"/>
-      <c r="T2" s="163"/>
+      <c r="N2" s="162"/>
+      <c r="O2" s="162"/>
+      <c r="P2" s="162"/>
+      <c r="Q2" s="162"/>
+      <c r="R2" s="162"/>
+      <c r="S2" s="162"/>
+      <c r="T2" s="162"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
@@ -3557,10 +3582,10 @@
       </c>
     </row>
     <row r="4" spans="1:20" s="149" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="165" t="s">
+      <c r="A4" s="164" t="s">
         <v>168</v>
       </c>
-      <c r="B4" s="165"/>
+      <c r="B4" s="164"/>
       <c r="G4" s="149" t="s">
         <v>152</v>
       </c>
@@ -4179,13 +4204,13 @@
     </row>
     <row r="38" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C39" s="163"/>
-      <c r="D39" s="163"/>
-      <c r="E39" s="163"/>
-      <c r="F39" s="163"/>
-      <c r="G39" s="163"/>
-      <c r="H39" s="163"/>
-      <c r="I39" s="163"/>
+      <c r="C39" s="162"/>
+      <c r="D39" s="162"/>
+      <c r="E39" s="162"/>
+      <c r="F39" s="162"/>
+      <c r="G39" s="162"/>
+      <c r="H39" s="162"/>
+      <c r="I39" s="162"/>
     </row>
     <row r="40" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4250,7 +4275,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF00FF"/>
   </sheetPr>
@@ -4258,7 +4283,7 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4296,17 +4321,17 @@
       <c r="K2" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
-      <c r="P2" s="163"/>
-      <c r="Q2" s="163"/>
-      <c r="R2" s="163"/>
-      <c r="S2" s="163"/>
-      <c r="T2" s="163"/>
+      <c r="N2" s="162"/>
+      <c r="O2" s="162"/>
+      <c r="P2" s="162"/>
+      <c r="Q2" s="162"/>
+      <c r="R2" s="162"/>
+      <c r="S2" s="162"/>
+      <c r="T2" s="162"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="166"/>
-      <c r="B3" s="166"/>
+      <c r="A3" s="165"/>
+      <c r="B3" s="165"/>
       <c r="D3" s="38" t="s">
         <v>146</v>
       </c>
@@ -4315,10 +4340,10 @@
       </c>
     </row>
     <row r="4" spans="1:20" s="149" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="165" t="s">
+      <c r="A4" s="164" t="s">
         <v>168</v>
       </c>
-      <c r="B4" s="165"/>
+      <c r="B4" s="164"/>
       <c r="J4" s="149" t="s">
         <v>169</v>
       </c>
@@ -4862,13 +4887,13 @@
       <c r="H37" s="110"/>
     </row>
     <row r="38" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C38" s="163"/>
-      <c r="D38" s="163"/>
-      <c r="E38" s="163"/>
-      <c r="F38" s="163"/>
-      <c r="G38" s="163"/>
-      <c r="H38" s="163"/>
-      <c r="I38" s="163"/>
+      <c r="C38" s="162"/>
+      <c r="D38" s="162"/>
+      <c r="E38" s="162"/>
+      <c r="F38" s="162"/>
+      <c r="G38" s="162"/>
+      <c r="H38" s="162"/>
+      <c r="I38" s="162"/>
     </row>
     <row r="39" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4935,7 +4960,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:T90"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -4979,13 +5004,13 @@
       <c r="K2" s="117">
         <v>180220042102</v>
       </c>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
-      <c r="P2" s="163"/>
-      <c r="Q2" s="163"/>
-      <c r="R2" s="163"/>
-      <c r="S2" s="163"/>
-      <c r="T2" s="163"/>
+      <c r="N2" s="162"/>
+      <c r="O2" s="162"/>
+      <c r="P2" s="162"/>
+      <c r="Q2" s="162"/>
+      <c r="R2" s="162"/>
+      <c r="S2" s="162"/>
+      <c r="T2" s="162"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" s="118"/>
@@ -4995,8 +5020,8 @@
       <c r="H3" s="118"/>
     </row>
     <row r="4" spans="1:20" s="118" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="167"/>
-      <c r="B4" s="167"/>
+      <c r="A4" s="166"/>
+      <c r="B4" s="166"/>
       <c r="D4" s="118" t="s">
         <v>179</v>
       </c>
@@ -5568,13 +5593,13 @@
     </row>
     <row r="38" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C39" s="163"/>
-      <c r="D39" s="163"/>
-      <c r="E39" s="163"/>
-      <c r="F39" s="163"/>
-      <c r="G39" s="163"/>
-      <c r="H39" s="163"/>
-      <c r="I39" s="163"/>
+      <c r="C39" s="162"/>
+      <c r="D39" s="162"/>
+      <c r="E39" s="162"/>
+      <c r="F39" s="162"/>
+      <c r="G39" s="162"/>
+      <c r="H39" s="162"/>
+      <c r="I39" s="162"/>
     </row>
     <row r="40" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5639,7 +5664,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -5685,13 +5710,13 @@
       <c r="K2" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
-      <c r="P2" s="163"/>
-      <c r="Q2" s="163"/>
-      <c r="R2" s="163"/>
-      <c r="S2" s="163"/>
-      <c r="T2" s="163"/>
+      <c r="N2" s="162"/>
+      <c r="O2" s="162"/>
+      <c r="P2" s="162"/>
+      <c r="Q2" s="162"/>
+      <c r="R2" s="162"/>
+      <c r="S2" s="162"/>
+      <c r="T2" s="162"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
@@ -6218,13 +6243,13 @@
       <c r="H36" s="110"/>
     </row>
     <row r="37" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C37" s="163"/>
-      <c r="D37" s="163"/>
-      <c r="E37" s="163"/>
-      <c r="F37" s="163"/>
-      <c r="G37" s="163"/>
-      <c r="H37" s="163"/>
-      <c r="I37" s="163"/>
+      <c r="C37" s="162"/>
+      <c r="D37" s="162"/>
+      <c r="E37" s="162"/>
+      <c r="F37" s="162"/>
+      <c r="G37" s="162"/>
+      <c r="H37" s="162"/>
+      <c r="I37" s="162"/>
     </row>
     <row r="38" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6289,7 +6314,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -6797,7 +6822,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -7347,7 +7372,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -8214,7 +8239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -8977,7 +9002,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -9021,13 +9046,13 @@
       <c r="K2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
-      <c r="P2" s="163"/>
-      <c r="Q2" s="163"/>
-      <c r="R2" s="163"/>
-      <c r="S2" s="163"/>
-      <c r="T2" s="163"/>
+      <c r="N2" s="162"/>
+      <c r="O2" s="162"/>
+      <c r="P2" s="162"/>
+      <c r="Q2" s="162"/>
+      <c r="R2" s="162"/>
+      <c r="S2" s="162"/>
+      <c r="T2" s="162"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
@@ -9619,13 +9644,13 @@
     </row>
     <row r="36" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C37" s="163"/>
-      <c r="D37" s="163"/>
-      <c r="E37" s="163"/>
-      <c r="F37" s="163"/>
-      <c r="G37" s="163"/>
-      <c r="H37" s="163"/>
-      <c r="I37" s="163"/>
+      <c r="C37" s="162"/>
+      <c r="D37" s="162"/>
+      <c r="E37" s="162"/>
+      <c r="F37" s="162"/>
+      <c r="G37" s="162"/>
+      <c r="H37" s="162"/>
+      <c r="I37" s="162"/>
     </row>
     <row r="38" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9690,7 +9715,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -9733,13 +9758,13 @@
       <c r="K2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
-      <c r="P2" s="163"/>
-      <c r="Q2" s="163"/>
-      <c r="R2" s="163"/>
-      <c r="S2" s="163"/>
-      <c r="T2" s="163"/>
+      <c r="N2" s="162"/>
+      <c r="O2" s="162"/>
+      <c r="P2" s="162"/>
+      <c r="Q2" s="162"/>
+      <c r="R2" s="162"/>
+      <c r="S2" s="162"/>
+      <c r="T2" s="162"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
@@ -10319,13 +10344,13 @@
     </row>
     <row r="36" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C37" s="163"/>
-      <c r="D37" s="163"/>
-      <c r="E37" s="163"/>
-      <c r="F37" s="163"/>
-      <c r="G37" s="163"/>
-      <c r="H37" s="163"/>
-      <c r="I37" s="163"/>
+      <c r="C37" s="162"/>
+      <c r="D37" s="162"/>
+      <c r="E37" s="162"/>
+      <c r="F37" s="162"/>
+      <c r="G37" s="162"/>
+      <c r="H37" s="162"/>
+      <c r="I37" s="162"/>
     </row>
     <row r="38" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10388,7 +10413,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -10434,13 +10459,13 @@
       <c r="K2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
-      <c r="P2" s="163"/>
-      <c r="Q2" s="163"/>
-      <c r="R2" s="163"/>
-      <c r="S2" s="163"/>
-      <c r="T2" s="163"/>
+      <c r="N2" s="162"/>
+      <c r="O2" s="162"/>
+      <c r="P2" s="162"/>
+      <c r="Q2" s="162"/>
+      <c r="R2" s="162"/>
+      <c r="S2" s="162"/>
+      <c r="T2" s="162"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
@@ -11008,13 +11033,13 @@
       <c r="H36" s="110"/>
     </row>
     <row r="37" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C37" s="163"/>
-      <c r="D37" s="163"/>
-      <c r="E37" s="163"/>
-      <c r="F37" s="163"/>
-      <c r="G37" s="163"/>
-      <c r="H37" s="163"/>
-      <c r="I37" s="163"/>
+      <c r="C37" s="162"/>
+      <c r="D37" s="162"/>
+      <c r="E37" s="162"/>
+      <c r="F37" s="162"/>
+      <c r="G37" s="162"/>
+      <c r="H37" s="162"/>
+      <c r="I37" s="162"/>
     </row>
     <row r="38" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11079,7 +11104,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -11124,13 +11149,13 @@
       <c r="K2" s="117">
         <v>160526021905</v>
       </c>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
-      <c r="P2" s="163"/>
-      <c r="Q2" s="163"/>
-      <c r="R2" s="163"/>
-      <c r="S2" s="163"/>
-      <c r="T2" s="163"/>
+      <c r="N2" s="162"/>
+      <c r="O2" s="162"/>
+      <c r="P2" s="162"/>
+      <c r="Q2" s="162"/>
+      <c r="R2" s="162"/>
+      <c r="S2" s="162"/>
+      <c r="T2" s="162"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
@@ -11718,13 +11743,13 @@
     </row>
     <row r="35" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="36" spans="2:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C36" s="163"/>
-      <c r="D36" s="163"/>
-      <c r="E36" s="163"/>
-      <c r="F36" s="163"/>
-      <c r="G36" s="163"/>
-      <c r="H36" s="163"/>
-      <c r="I36" s="163"/>
+      <c r="C36" s="162"/>
+      <c r="D36" s="162"/>
+      <c r="E36" s="162"/>
+      <c r="F36" s="162"/>
+      <c r="G36" s="162"/>
+      <c r="H36" s="162"/>
+      <c r="I36" s="162"/>
     </row>
     <row r="37" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
ready for client reviw to fix some details and get the expected behavior, 0cells appear to have some non cero values but very close to 0, should we round to 0?, some binLocation numbers are not found in its worksheets
</commit_message>
<xml_diff>
--- a/files/A01-101 APT Agar.xlsx
+++ b/files/A01-101 APT Agar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D1FADF-44DF-4F89-8BFF-55D83A6B82CB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CFE1F7-D06F-42AA-85FC-3980A00A3808}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="420" windowWidth="15465" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="191">
   <si>
     <t>.</t>
   </si>
@@ -609,16 +609,10 @@
     <t>A01-101-A</t>
   </si>
   <si>
-    <t>Bulk-3M</t>
-  </si>
-  <si>
     <t>A01-101-3M</t>
   </si>
   <si>
     <t>A01-101-C</t>
-  </si>
-  <si>
-    <t>Bulk-Other</t>
   </si>
   <si>
     <t>3M 2.5 kg 
@@ -1293,6 +1287,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1307,9 +1304,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1656,7 +1650,7 @@
   <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1694,25 +1688,25 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D3" t="s">
         <v>183</v>
       </c>
       <c r="E3" s="161" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G3" t="s">
+        <v>189</v>
+      </c>
+      <c r="H3" t="s">
         <v>190</v>
       </c>
-      <c r="G3" t="s">
-        <v>191</v>
-      </c>
-      <c r="H3" t="s">
-        <v>192</v>
-      </c>
       <c r="L3" s="51" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M3" s="51" t="s">
         <v>14</v>
@@ -1740,8 +1734,8 @@
       <c r="G4" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="167" t="s">
-        <v>188</v>
+      <c r="H4" s="162" t="s">
+        <v>186</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>9</v>
@@ -1750,10 +1744,10 @@
         <v>9</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>184</v>
+        <v>4</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>187</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2908,13 +2902,13 @@
       <c r="K2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="N2" s="162"/>
-      <c r="O2" s="162"/>
-      <c r="P2" s="162"/>
-      <c r="Q2" s="162"/>
-      <c r="R2" s="162"/>
-      <c r="S2" s="162"/>
-      <c r="T2" s="162"/>
+      <c r="N2" s="163"/>
+      <c r="O2" s="163"/>
+      <c r="P2" s="163"/>
+      <c r="Q2" s="163"/>
+      <c r="R2" s="163"/>
+      <c r="S2" s="163"/>
+      <c r="T2" s="163"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
@@ -2925,10 +2919,10 @@
       </c>
     </row>
     <row r="4" spans="1:20" s="149" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="163" t="s">
+      <c r="A4" s="164" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="163"/>
+      <c r="B4" s="164"/>
     </row>
     <row r="5" spans="1:20" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="97" t="s">
@@ -3554,13 +3548,13 @@
       <c r="K2" s="117">
         <v>161228021912</v>
       </c>
-      <c r="N2" s="162"/>
-      <c r="O2" s="162"/>
-      <c r="P2" s="162"/>
-      <c r="Q2" s="162"/>
-      <c r="R2" s="162"/>
-      <c r="S2" s="162"/>
-      <c r="T2" s="162"/>
+      <c r="N2" s="163"/>
+      <c r="O2" s="163"/>
+      <c r="P2" s="163"/>
+      <c r="Q2" s="163"/>
+      <c r="R2" s="163"/>
+      <c r="S2" s="163"/>
+      <c r="T2" s="163"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
@@ -3582,10 +3576,10 @@
       </c>
     </row>
     <row r="4" spans="1:20" s="149" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="164" t="s">
+      <c r="A4" s="165" t="s">
         <v>168</v>
       </c>
-      <c r="B4" s="164"/>
+      <c r="B4" s="165"/>
       <c r="G4" s="149" t="s">
         <v>152</v>
       </c>
@@ -4204,13 +4198,13 @@
     </row>
     <row r="38" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C39" s="162"/>
-      <c r="D39" s="162"/>
-      <c r="E39" s="162"/>
-      <c r="F39" s="162"/>
-      <c r="G39" s="162"/>
-      <c r="H39" s="162"/>
-      <c r="I39" s="162"/>
+      <c r="C39" s="163"/>
+      <c r="D39" s="163"/>
+      <c r="E39" s="163"/>
+      <c r="F39" s="163"/>
+      <c r="G39" s="163"/>
+      <c r="H39" s="163"/>
+      <c r="I39" s="163"/>
     </row>
     <row r="40" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4321,17 +4315,17 @@
       <c r="K2" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="N2" s="162"/>
-      <c r="O2" s="162"/>
-      <c r="P2" s="162"/>
-      <c r="Q2" s="162"/>
-      <c r="R2" s="162"/>
-      <c r="S2" s="162"/>
-      <c r="T2" s="162"/>
+      <c r="N2" s="163"/>
+      <c r="O2" s="163"/>
+      <c r="P2" s="163"/>
+      <c r="Q2" s="163"/>
+      <c r="R2" s="163"/>
+      <c r="S2" s="163"/>
+      <c r="T2" s="163"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="165"/>
-      <c r="B3" s="165"/>
+      <c r="A3" s="166"/>
+      <c r="B3" s="166"/>
       <c r="D3" s="38" t="s">
         <v>146</v>
       </c>
@@ -4340,10 +4334,10 @@
       </c>
     </row>
     <row r="4" spans="1:20" s="149" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="164" t="s">
+      <c r="A4" s="165" t="s">
         <v>168</v>
       </c>
-      <c r="B4" s="164"/>
+      <c r="B4" s="165"/>
       <c r="J4" s="149" t="s">
         <v>169</v>
       </c>
@@ -4887,13 +4881,13 @@
       <c r="H37" s="110"/>
     </row>
     <row r="38" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C38" s="162"/>
-      <c r="D38" s="162"/>
-      <c r="E38" s="162"/>
-      <c r="F38" s="162"/>
-      <c r="G38" s="162"/>
-      <c r="H38" s="162"/>
-      <c r="I38" s="162"/>
+      <c r="C38" s="163"/>
+      <c r="D38" s="163"/>
+      <c r="E38" s="163"/>
+      <c r="F38" s="163"/>
+      <c r="G38" s="163"/>
+      <c r="H38" s="163"/>
+      <c r="I38" s="163"/>
     </row>
     <row r="39" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5004,13 +4998,13 @@
       <c r="K2" s="117">
         <v>180220042102</v>
       </c>
-      <c r="N2" s="162"/>
-      <c r="O2" s="162"/>
-      <c r="P2" s="162"/>
-      <c r="Q2" s="162"/>
-      <c r="R2" s="162"/>
-      <c r="S2" s="162"/>
-      <c r="T2" s="162"/>
+      <c r="N2" s="163"/>
+      <c r="O2" s="163"/>
+      <c r="P2" s="163"/>
+      <c r="Q2" s="163"/>
+      <c r="R2" s="163"/>
+      <c r="S2" s="163"/>
+      <c r="T2" s="163"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" s="118"/>
@@ -5020,8 +5014,8 @@
       <c r="H3" s="118"/>
     </row>
     <row r="4" spans="1:20" s="118" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="166"/>
-      <c r="B4" s="166"/>
+      <c r="A4" s="167"/>
+      <c r="B4" s="167"/>
       <c r="D4" s="118" t="s">
         <v>179</v>
       </c>
@@ -5593,13 +5587,13 @@
     </row>
     <row r="38" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C39" s="162"/>
-      <c r="D39" s="162"/>
-      <c r="E39" s="162"/>
-      <c r="F39" s="162"/>
-      <c r="G39" s="162"/>
-      <c r="H39" s="162"/>
-      <c r="I39" s="162"/>
+      <c r="C39" s="163"/>
+      <c r="D39" s="163"/>
+      <c r="E39" s="163"/>
+      <c r="F39" s="163"/>
+      <c r="G39" s="163"/>
+      <c r="H39" s="163"/>
+      <c r="I39" s="163"/>
     </row>
     <row r="40" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5710,13 +5704,13 @@
       <c r="K2" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="N2" s="162"/>
-      <c r="O2" s="162"/>
-      <c r="P2" s="162"/>
-      <c r="Q2" s="162"/>
-      <c r="R2" s="162"/>
-      <c r="S2" s="162"/>
-      <c r="T2" s="162"/>
+      <c r="N2" s="163"/>
+      <c r="O2" s="163"/>
+      <c r="P2" s="163"/>
+      <c r="Q2" s="163"/>
+      <c r="R2" s="163"/>
+      <c r="S2" s="163"/>
+      <c r="T2" s="163"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
@@ -6243,13 +6237,13 @@
       <c r="H36" s="110"/>
     </row>
     <row r="37" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C37" s="162"/>
-      <c r="D37" s="162"/>
-      <c r="E37" s="162"/>
-      <c r="F37" s="162"/>
-      <c r="G37" s="162"/>
-      <c r="H37" s="162"/>
-      <c r="I37" s="162"/>
+      <c r="C37" s="163"/>
+      <c r="D37" s="163"/>
+      <c r="E37" s="163"/>
+      <c r="F37" s="163"/>
+      <c r="G37" s="163"/>
+      <c r="H37" s="163"/>
+      <c r="I37" s="163"/>
     </row>
     <row r="38" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9046,13 +9040,13 @@
       <c r="K2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="N2" s="162"/>
-      <c r="O2" s="162"/>
-      <c r="P2" s="162"/>
-      <c r="Q2" s="162"/>
-      <c r="R2" s="162"/>
-      <c r="S2" s="162"/>
-      <c r="T2" s="162"/>
+      <c r="N2" s="163"/>
+      <c r="O2" s="163"/>
+      <c r="P2" s="163"/>
+      <c r="Q2" s="163"/>
+      <c r="R2" s="163"/>
+      <c r="S2" s="163"/>
+      <c r="T2" s="163"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
@@ -9644,13 +9638,13 @@
     </row>
     <row r="36" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C37" s="162"/>
-      <c r="D37" s="162"/>
-      <c r="E37" s="162"/>
-      <c r="F37" s="162"/>
-      <c r="G37" s="162"/>
-      <c r="H37" s="162"/>
-      <c r="I37" s="162"/>
+      <c r="C37" s="163"/>
+      <c r="D37" s="163"/>
+      <c r="E37" s="163"/>
+      <c r="F37" s="163"/>
+      <c r="G37" s="163"/>
+      <c r="H37" s="163"/>
+      <c r="I37" s="163"/>
     </row>
     <row r="38" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9758,13 +9752,13 @@
       <c r="K2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="N2" s="162"/>
-      <c r="O2" s="162"/>
-      <c r="P2" s="162"/>
-      <c r="Q2" s="162"/>
-      <c r="R2" s="162"/>
-      <c r="S2" s="162"/>
-      <c r="T2" s="162"/>
+      <c r="N2" s="163"/>
+      <c r="O2" s="163"/>
+      <c r="P2" s="163"/>
+      <c r="Q2" s="163"/>
+      <c r="R2" s="163"/>
+      <c r="S2" s="163"/>
+      <c r="T2" s="163"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
@@ -10344,13 +10338,13 @@
     </row>
     <row r="36" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C37" s="162"/>
-      <c r="D37" s="162"/>
-      <c r="E37" s="162"/>
-      <c r="F37" s="162"/>
-      <c r="G37" s="162"/>
-      <c r="H37" s="162"/>
-      <c r="I37" s="162"/>
+      <c r="C37" s="163"/>
+      <c r="D37" s="163"/>
+      <c r="E37" s="163"/>
+      <c r="F37" s="163"/>
+      <c r="G37" s="163"/>
+      <c r="H37" s="163"/>
+      <c r="I37" s="163"/>
     </row>
     <row r="38" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10459,13 +10453,13 @@
       <c r="K2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="N2" s="162"/>
-      <c r="O2" s="162"/>
-      <c r="P2" s="162"/>
-      <c r="Q2" s="162"/>
-      <c r="R2" s="162"/>
-      <c r="S2" s="162"/>
-      <c r="T2" s="162"/>
+      <c r="N2" s="163"/>
+      <c r="O2" s="163"/>
+      <c r="P2" s="163"/>
+      <c r="Q2" s="163"/>
+      <c r="R2" s="163"/>
+      <c r="S2" s="163"/>
+      <c r="T2" s="163"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
@@ -11033,13 +11027,13 @@
       <c r="H36" s="110"/>
     </row>
     <row r="37" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C37" s="162"/>
-      <c r="D37" s="162"/>
-      <c r="E37" s="162"/>
-      <c r="F37" s="162"/>
-      <c r="G37" s="162"/>
-      <c r="H37" s="162"/>
-      <c r="I37" s="162"/>
+      <c r="C37" s="163"/>
+      <c r="D37" s="163"/>
+      <c r="E37" s="163"/>
+      <c r="F37" s="163"/>
+      <c r="G37" s="163"/>
+      <c r="H37" s="163"/>
+      <c r="I37" s="163"/>
     </row>
     <row r="38" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11149,13 +11143,13 @@
       <c r="K2" s="117">
         <v>160526021905</v>
       </c>
-      <c r="N2" s="162"/>
-      <c r="O2" s="162"/>
-      <c r="P2" s="162"/>
-      <c r="Q2" s="162"/>
-      <c r="R2" s="162"/>
-      <c r="S2" s="162"/>
-      <c r="T2" s="162"/>
+      <c r="N2" s="163"/>
+      <c r="O2" s="163"/>
+      <c r="P2" s="163"/>
+      <c r="Q2" s="163"/>
+      <c r="R2" s="163"/>
+      <c r="S2" s="163"/>
+      <c r="T2" s="163"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
@@ -11743,13 +11737,13 @@
     </row>
     <row r="35" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="36" spans="2:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C36" s="162"/>
-      <c r="D36" s="162"/>
-      <c r="E36" s="162"/>
-      <c r="F36" s="162"/>
-      <c r="G36" s="162"/>
-      <c r="H36" s="162"/>
-      <c r="I36" s="162"/>
+      <c r="C36" s="163"/>
+      <c r="D36" s="163"/>
+      <c r="E36" s="163"/>
+      <c r="F36" s="163"/>
+      <c r="G36" s="163"/>
+      <c r="H36" s="163"/>
+      <c r="I36" s="163"/>
     </row>
     <row r="37" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>